<commit_message>
maj des sfd creation classe MlIdentification
</commit_message>
<xml_diff>
--- a/CarnetVet/trunk/documentation/sfd.xlsx
+++ b/CarnetVet/trunk/documentation/sfd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="11715" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="11715" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Objets" sheetId="1" r:id="rId1"/>
@@ -15,23 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
   <si>
     <t>MlCarnet</t>
   </si>
   <si>
-    <t>MlIdentification</t>
-  </si>
-  <si>
     <t>Nom</t>
   </si>
   <si>
-    <t>DateNaissance</t>
-  </si>
-  <si>
-    <t>AgeCalcule</t>
-  </si>
-  <si>
     <t>EnTypeAnimal</t>
   </si>
   <si>
@@ -339,6 +330,30 @@
   </si>
   <si>
     <t>TRAITEMENT</t>
+  </si>
+  <si>
+    <t>MlIdentificationAnimal</t>
+  </si>
+  <si>
+    <t>nomAnimal</t>
+  </si>
+  <si>
+    <t>dateNaissance</t>
+  </si>
+  <si>
+    <t>ageCalcule</t>
+  </si>
+  <si>
+    <t>typeAnimal</t>
+  </si>
+  <si>
+    <t>genreAnimal</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>identificationAnimal</t>
   </si>
 </sst>
 </file>
@@ -425,35 +440,35 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -752,14 +767,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -769,611 +784,632 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="13"/>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="13"/>
+      <c r="B4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="13" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="13" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="13"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="13"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="13"/>
+      <c r="B44" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="13"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="13"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="13"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="15" t="s">
+    <row r="48" spans="1:5">
+      <c r="A48" s="13"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="13"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="13"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="13"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="13"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="13"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="13"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="13"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="13"/>
+      <c r="B56" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="13"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="13"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="13"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="15" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" s="13"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="13"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="13"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="13"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="13"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="13"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="13"/>
+      <c r="B66" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="13"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="13"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="13"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" t="s">
+    <row r="70" spans="1:5">
+      <c r="A70" s="13"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="2"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="2"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2"/>
-      <c r="B44" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="2"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="2"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="2"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="2"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="2"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="7" t="s">
+    <row r="71" spans="1:5">
+      <c r="A71" s="13"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="13"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="13"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="2"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="2"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E55" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="2"/>
-      <c r="B56" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="2"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="2"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="2"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="2"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="2"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="2"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="2"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="2"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="2"/>
-      <c r="B66" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="2"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="2"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="2"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="2"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="2"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="9" t="s">
+    <row r="74" spans="1:5">
+      <c r="A74" s="13"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="5" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="2"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="2"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E73" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="2"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C17:C43"/>
+    <mergeCell ref="C68:C74"/>
+    <mergeCell ref="A2:A74"/>
+    <mergeCell ref="B5:B43"/>
+    <mergeCell ref="B45:B55"/>
+    <mergeCell ref="B57:B65"/>
+    <mergeCell ref="B67:B74"/>
     <mergeCell ref="D24:D29"/>
     <mergeCell ref="D31:D36"/>
     <mergeCell ref="D38:D43"/>
@@ -1381,15 +1417,6 @@
     <mergeCell ref="C58:C65"/>
     <mergeCell ref="D63:D64"/>
     <mergeCell ref="D50:D54"/>
-    <mergeCell ref="A2:A74"/>
-    <mergeCell ref="B5:B43"/>
-    <mergeCell ref="B45:B55"/>
-    <mergeCell ref="B57:B65"/>
-    <mergeCell ref="B67:B74"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C17:C43"/>
-    <mergeCell ref="C68:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1399,7 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1412,438 +1439,438 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="B21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="B22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="B24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="B27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="B28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="B29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="B35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="B36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="B37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="B42" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="B45" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="B46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="B50" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="B51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="B52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="B53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="B54" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="B55" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="B56" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>